<commit_message>
Rregullimi final i responsivness
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1067,16 +1067,33 @@
         <v>rr. 101 pn</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40">
+        <v>28</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Test1</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Test2</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Amviseri</v>
+      </c>
+      <c r="E40" t="str">
+        <v>rrrr</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E40"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1242,9 +1259,32 @@
         <v>99.5</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2025-06-17T09:06:04.199Z</v>
+      </c>
+      <c r="D8">
+        <v>153</v>
+      </c>
+      <c r="E8">
+        <v>174</v>
+      </c>
+      <c r="F8">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>10.5</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Buttoni TOP ne faqet consumers, history dhe readings
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -1093,7 +1093,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1282,9 +1282,170 @@
         <v>10.5</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-06-17T10:48:25.637Z</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-06-17T10:48:32.842Z</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>52</v>
+      </c>
+      <c r="F10">
+        <v>52</v>
+      </c>
+      <c r="G10">
+        <v>62.4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2025-06-17T10:48:38.621Z</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>74</v>
+      </c>
+      <c r="F11">
+        <v>74</v>
+      </c>
+      <c r="G11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2025-06-17T10:48:56.958Z</v>
+      </c>
+      <c r="D12">
+        <v>199</v>
+      </c>
+      <c r="E12">
+        <v>207</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2025-06-17T10:49:02.956Z</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2025-06-17T10:49:09.165Z</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>56</v>
+      </c>
+      <c r="G14">
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>26</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2025-06-17T10:49:44.465Z</v>
+      </c>
+      <c r="D15">
+        <v>56</v>
+      </c>
+      <c r="E15">
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <v>18</v>
+      </c>
+      <c r="G15">
+        <v>21.599999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G15"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
rregullimi i test users dhe dashboard css
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AliMunishiApp\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC83C65-B191-45F0-9F67-1727AAA1BD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAB401E-02BA-4FCE-9816-274DBAF7785C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="consumers" sheetId="1" r:id="rId1"/>
@@ -832,11 +832,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -870,7 +872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -887,7 +889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -904,7 +906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -921,7 +923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18</v>
       </c>
@@ -938,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>19</v>
       </c>
@@ -955,7 +957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -972,7 +974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>21</v>
       </c>
@@ -989,7 +991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22</v>
       </c>
@@ -1006,7 +1008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>23</v>
       </c>
@@ -1023,7 +1025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>24</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
@@ -1057,7 +1059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
@@ -1074,9 +1076,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -1091,9 +1093,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -1108,9 +1110,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
@@ -1125,9 +1127,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>49</v>
@@ -1142,9 +1144,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>52</v>
@@ -1159,9 +1161,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
@@ -1176,9 +1178,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
@@ -1193,9 +1195,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
@@ -1210,9 +1212,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
@@ -1227,9 +1229,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>67</v>
@@ -1244,9 +1246,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
@@ -1261,9 +1263,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
@@ -1278,9 +1280,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
@@ -1295,9 +1297,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>79</v>
@@ -1312,9 +1314,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
@@ -1329,9 +1331,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>85</v>
@@ -1346,9 +1348,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
@@ -1363,9 +1365,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
         <v>91</v>
@@ -1380,9 +1382,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
         <v>94</v>
@@ -1397,9 +1399,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
         <v>97</v>
@@ -1414,9 +1416,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
         <v>100</v>
@@ -1431,9 +1433,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
         <v>103</v>
@@ -1448,9 +1450,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
         <v>106</v>
@@ -1465,9 +1467,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
         <v>109</v>
@@ -1482,9 +1484,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
@@ -1499,9 +1501,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
         <v>114</v>
@@ -1519,7 +1521,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E40" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E13 B14:E40" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1530,9 +1532,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1601,7 +1607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1624,7 +1630,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1647,7 +1653,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>99.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1716,7 +1722,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1739,7 +1745,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>62.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1785,7 +1791,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1854,7 +1860,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1889,11 +1895,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>